<commit_message>
"Thêm alert check trường thông tin nhập toa thuốc và sửa các lastIndex nếu danh sách rỗng"
</commit_message>
<xml_diff>
--- a/Prj2/save/QLTuThuoc.xlsx
+++ b/Prj2/save/QLTuThuoc.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357568" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357719" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -261,6 +261,24 @@
   </si>
   <si>
     <t>adsf</t>
+  </si>
+  <si>
+    <t>Toa thuốc số 1</t>
+  </si>
+  <si>
+    <t>1 viên 1 ngày sau ăn</t>
+  </si>
+  <si>
+    <t>Toa thuốc chữa trĩ cho Hồng</t>
+  </si>
+  <si>
+    <t>1 viên 1 ngày</t>
+  </si>
+  <si>
+    <t>Toa thuốc cho Riêu</t>
+  </si>
+  <si>
+    <t>150ml 1 ngày</t>
   </si>
 </sst>
 </file>
@@ -316,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
@@ -325,6 +343,12 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -672,7 +696,7 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="78" t="n">
+      <c r="F2" s="84" t="n">
         <v>45005.0</v>
       </c>
     </row>
@@ -692,7 +716,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="78" t="n">
+      <c r="F3" s="84" t="n">
         <v>44757.0</v>
       </c>
     </row>
@@ -712,7 +736,7 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="78" t="n">
+      <c r="F4" s="84" t="n">
         <v>45000.0</v>
       </c>
     </row>
@@ -732,7 +756,7 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="78" t="n">
+      <c r="F5" s="84" t="n">
         <v>45119.0</v>
       </c>
     </row>
@@ -752,7 +776,7 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="78" t="n">
+      <c r="F6" s="84" t="n">
         <v>44757.0</v>
       </c>
     </row>
@@ -772,7 +796,7 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="78" t="n">
+      <c r="F7" s="84" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -792,7 +816,7 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="78" t="n">
+      <c r="F8" s="84" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -812,7 +836,7 @@
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="78" t="n">
+      <c r="F9" s="84" t="n">
         <v>45000.0</v>
       </c>
     </row>
@@ -832,7 +856,7 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="78" t="n">
+      <c r="F10" s="84" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -852,7 +876,7 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="78" t="n">
+      <c r="F11" s="84" t="n">
         <v>45005.0</v>
       </c>
     </row>
@@ -872,7 +896,7 @@
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="78" t="n">
+      <c r="F12" s="84" t="n">
         <v>44772.0</v>
       </c>
     </row>
@@ -887,7 +911,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -918,13 +942,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="n" s="79">
-        <v>44764.0</v>
-      </c>
-      <c r="D2" t="n" s="79">
-        <v>44739.0</v>
+        <v>75</v>
+      </c>
+      <c r="C2" t="n" s="85">
+        <v>44757.0</v>
+      </c>
+      <c r="D2" t="n" s="85">
+        <v>44755.0</v>
       </c>
     </row>
     <row r="3">
@@ -932,13 +956,27 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="n" s="79">
-        <v>44741.0</v>
-      </c>
-      <c r="D3" t="n" s="79">
-        <v>44740.0</v>
+        <v>77</v>
+      </c>
+      <c r="C3" t="n" s="85">
+        <v>44751.0</v>
+      </c>
+      <c r="D3" t="n" s="85">
+        <v>44745.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="n" s="85">
+        <v>44761.0</v>
+      </c>
+      <c r="D4" t="n" s="85">
+        <v>44757.0</v>
       </c>
     </row>
   </sheetData>
@@ -1015,7 +1053,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD14"/>
@@ -1045,13 +1083,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E2" t="n">
         <v>1.0</v>
@@ -1062,16 +1100,33 @@
         <v>1.0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="E3" t="n">
         <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>